<commit_message>
updated .ignore, implemented interfaces
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work\Projects\.NET\HelloWorldApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2521DB0A-30CD-49B9-80FC-4C5AF5F53067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB1016F-6C58-437B-B6D6-2B47588C5845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -147,9 +147,6 @@
     <t>goal: lv2 start</t>
   </si>
   <si>
-    <t>goal: #230 start  ---- currently: 85</t>
-  </si>
-  <si>
     <t xml:space="preserve">goal: #390 start </t>
   </si>
   <si>
@@ -169,6 +166,9 @@
   </si>
   <si>
     <t>goal: lv4: start</t>
+  </si>
+  <si>
+    <t>goal: #230 start  ---- currently: 90</t>
   </si>
 </sst>
 </file>
@@ -189,7 +189,7 @@
       <name val="Cascadia Code"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,6 +220,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -518,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -581,11 +587,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -596,26 +600,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -893,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.42578125" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -958,7 +954,7 @@
       <c r="E3" s="22">
         <v>2</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="12" t="s">
         <v>33</v>
       </c>
       <c r="G3" s="7"/>
@@ -971,13 +967,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="27"/>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="39" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="22">
         <v>3</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="32" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="7"/>
@@ -1008,8 +1004,8 @@
       <c r="B6" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37" t="s">
+      <c r="C6" s="35"/>
+      <c r="D6" s="35" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="24">
@@ -1023,25 +1019,25 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="20"/>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="38"/>
+      <c r="D7" s="36"/>
       <c r="E7" s="25"/>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="39" t="s">
+      <c r="C8" s="36"/>
+      <c r="D8" s="38" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="5"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="35"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="33"/>
       <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1073,12 +1069,12 @@
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="1" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1087,7 +1083,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>23</v>
@@ -1101,7 +1097,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>24</v>
@@ -1115,7 +1111,7 @@
         <v>25</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>25</v>
@@ -1129,7 +1125,7 @@
         <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>26</v>
@@ -1142,36 +1138,36 @@
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="40"/>
+      <c r="B17" s="37"/>
       <c r="E17" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="40"/>
+      <c r="B18" s="37"/>
       <c r="E18" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="40"/>
+      <c r="B19" s="37"/>
       <c r="E19" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1179,13 +1175,13 @@
         <v>30</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>30</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>